<commit_message>
V 1.0.4: Fix AGIP
</commit_message>
<xml_diff>
--- a/Control.xlsx
+++ b/Control.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin Bustos\Desktop\BOT RETPER IIBB ARBA AGIP\RETPER ARBA y AGIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757A8A56-50CF-4A3A-BCF5-351C3C77CC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B54137-944F-41EB-8F6C-E0AEF4789333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -398,7 +398,7 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="83.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="140" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>

</xml_diff>